<commit_message>
Prototip spajanja podataka na izbor 3
- odabir u izboru 3 spojen na pandas
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Vocnjaci</t>
+  </si>
+  <si>
+    <t>Zupanija</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -853,6 +856,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
@@ -1538,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1554,6 +1560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="6" t="s">
         <v>38</v>
       </c>

</xml_diff>